<commit_message>
Analysis & Prediction Page Completed
</commit_message>
<xml_diff>
--- a/AuraSite/App/Data/second.xlsx
+++ b/AuraSite/App/Data/second.xlsx
@@ -1249,294 +1249,294 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>2018-11-24 09_36 - Priyanka Mitra</t>
+          <t>2017-12-24 17_02 - Dr. Amit</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="n">
-        <v>2.71</v>
+        <v>2.32</v>
       </c>
       <c r="D4" t="n">
-        <v>54.38</v>
+        <v>60.28</v>
       </c>
       <c r="E4" t="n">
-        <v>99.23999999999999</v>
+        <v>97.41</v>
       </c>
       <c r="F4" t="n">
-        <v>91.26000000000001</v>
+        <v>92.95</v>
       </c>
       <c r="G4" t="n">
-        <v>2.38</v>
+        <v>2.61</v>
       </c>
       <c r="H4" t="n">
         <v>2.61</v>
       </c>
       <c r="I4" t="n">
-        <v>75013</v>
+        <v>81216</v>
       </c>
       <c r="J4" t="n">
-        <v>34.36</v>
+        <v>40.36</v>
       </c>
       <c r="K4" t="n">
-        <v>72405</v>
+        <v>78406</v>
       </c>
       <c r="L4" t="n">
-        <v>32.98</v>
+        <v>39.28</v>
       </c>
       <c r="M4" t="n">
-        <v>72868</v>
+        <v>82329</v>
       </c>
       <c r="N4" t="n">
-        <v>32.96</v>
+        <v>40.79</v>
       </c>
       <c r="O4" t="n">
-        <v>5.37</v>
+        <v>5.21</v>
       </c>
       <c r="P4" t="n">
+        <v>5.25</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>5.07</v>
+      </c>
+      <c r="R4" t="n">
+        <v>4.51</v>
+      </c>
+      <c r="S4" t="n">
+        <v>5.71</v>
+      </c>
+      <c r="T4" t="n">
+        <v>5.01</v>
+      </c>
+      <c r="U4" t="n">
         <v>4.99</v>
       </c>
-      <c r="Q4" t="n">
-        <v>5.52</v>
-      </c>
-      <c r="R4" t="n">
-        <v>5.09</v>
-      </c>
-      <c r="S4" t="n">
-        <v>5.72</v>
-      </c>
-      <c r="T4" t="n">
+      <c r="V4" t="n">
+        <v>92.31999999999999</v>
+      </c>
+      <c r="W4" t="n">
+        <v>79.12</v>
+      </c>
+      <c r="X4" t="n">
+        <v>93.67</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>98.93000000000001</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>92.47</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>98.73999999999999</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>96.09</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>-0.19</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>-0.23</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>93.05</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>79.20999999999999</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>50.05</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>49.95</v>
+      </c>
+      <c r="AN4" t="n">
         <v>4.8</v>
       </c>
-      <c r="U4" t="n">
-        <v>4.41</v>
-      </c>
-      <c r="V4" t="n">
-        <v>90.7</v>
-      </c>
-      <c r="W4" t="n">
-        <v>96.26000000000001</v>
-      </c>
-      <c r="X4" t="n">
-        <v>85.7</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>92.59999999999999</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>87.52</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>95.58</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>95.14</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>-0.28</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>-0.11</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>-0.43</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>-0.22</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>-0.37</v>
-      </c>
-      <c r="AH4" t="n">
-        <v>0.13</v>
-      </c>
-      <c r="AI4" t="n">
-        <v>-0.15</v>
-      </c>
-      <c r="AJ4" t="n">
-        <v>91.93000000000001</v>
-      </c>
-      <c r="AK4" t="n">
-        <v>78.59</v>
-      </c>
-      <c r="AL4" t="n">
-        <v>51.58</v>
-      </c>
-      <c r="AM4" t="n">
-        <v>48.42</v>
-      </c>
-      <c r="AN4" t="n">
-        <v>4.16</v>
-      </c>
       <c r="AO4" t="n">
-        <v>5.47</v>
+        <v>4.69</v>
       </c>
       <c r="AP4" t="n">
-        <v>7.07</v>
+        <v>4.25</v>
       </c>
       <c r="AQ4" t="n">
-        <v>5.37</v>
+        <v>6.33</v>
       </c>
       <c r="AR4" t="n">
-        <v>5.22</v>
+        <v>4.75</v>
       </c>
       <c r="AS4" t="n">
-        <v>4.67</v>
+        <v>5.84</v>
       </c>
       <c r="AT4" t="n">
-        <v>4.73</v>
+        <v>4.74</v>
       </c>
       <c r="AU4" t="n">
-        <v>4.74</v>
+        <v>5.12</v>
       </c>
       <c r="AV4" t="n">
-        <v>5.19</v>
+        <v>5.23</v>
       </c>
       <c r="AW4" t="n">
-        <v>5.51</v>
+        <v>5.34</v>
       </c>
       <c r="AX4" t="n">
-        <v>4.77</v>
+        <v>5.35</v>
       </c>
       <c r="AY4" t="n">
-        <v>5.06</v>
+        <v>4.84</v>
       </c>
       <c r="AZ4" t="n">
-        <v>4.97</v>
+        <v>5.74</v>
       </c>
       <c r="BA4" t="n">
-        <v>4.53</v>
+        <v>5.79</v>
       </c>
       <c r="BB4" t="n">
-        <v>4.88</v>
+        <v>3.82</v>
       </c>
       <c r="BC4" t="n">
-        <v>4.4</v>
+        <v>4.85</v>
       </c>
       <c r="BD4" t="n">
-        <v>4.67</v>
+        <v>5.84</v>
       </c>
       <c r="BE4" t="n">
-        <v>4.16</v>
+        <v>4.8</v>
       </c>
       <c r="BF4" t="n">
-        <v>4.49</v>
+        <v>4.45</v>
       </c>
       <c r="BG4" t="n">
         <v>4.29</v>
       </c>
       <c r="BH4" t="n">
-        <v>5.47</v>
+        <v>4.69</v>
       </c>
       <c r="BI4" t="n">
-        <v>4.69</v>
+        <v>4.97</v>
       </c>
       <c r="BJ4" t="n">
-        <v>4.77</v>
+        <v>5.35</v>
       </c>
       <c r="BK4" t="n">
-        <v>4.44</v>
+        <v>5.14</v>
       </c>
       <c r="BL4" t="n">
-        <v>4.17</v>
+        <v>4.57</v>
       </c>
       <c r="BM4" t="n">
-        <v>4.23</v>
+        <v>5.37</v>
       </c>
       <c r="BN4" t="n">
-        <v>5.88</v>
+        <v>5.27</v>
       </c>
       <c r="BO4" t="n">
-        <v>0</v>
+        <v>6.33</v>
       </c>
       <c r="BP4" t="n">
-        <v>4.66</v>
+        <v>5.24</v>
       </c>
       <c r="BQ4" t="n">
-        <v>0</v>
+        <v>5.52</v>
       </c>
       <c r="BR4" t="n">
-        <v>5.45</v>
+        <v>5</v>
       </c>
       <c r="BS4" t="n">
-        <v>4.38</v>
+        <v>4.89</v>
       </c>
       <c r="BT4" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="BU4" t="n">
+        <v>5.54</v>
+      </c>
+      <c r="BV4" t="n">
+        <v>4.97</v>
+      </c>
+      <c r="BW4" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="BX4" t="n">
+        <v>6.26</v>
+      </c>
+      <c r="BY4" t="n">
+        <v>5.55</v>
+      </c>
+      <c r="BZ4" t="n">
+        <v>4.79</v>
+      </c>
+      <c r="CA4" t="n">
+        <v>5.04</v>
+      </c>
+      <c r="CB4" t="n">
+        <v>5.39</v>
+      </c>
+      <c r="CC4" t="n">
+        <v>4.53</v>
+      </c>
+      <c r="CD4" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="CE4" t="n">
+        <v>4.98</v>
+      </c>
+      <c r="CF4" t="n">
         <v>4.63</v>
       </c>
-      <c r="BU4" t="n">
-        <v>5.42</v>
-      </c>
-      <c r="BV4" t="n">
-        <v>6.89</v>
-      </c>
-      <c r="BW4" t="n">
-        <v>5.15</v>
-      </c>
-      <c r="BX4" t="n">
-        <v>4.78</v>
-      </c>
-      <c r="BY4" t="n">
-        <v>4.76</v>
-      </c>
-      <c r="BZ4" t="n">
-        <v>4.71</v>
-      </c>
-      <c r="CA4" t="n">
-        <v>5.13</v>
-      </c>
-      <c r="CB4" t="n">
-        <v>5.02</v>
-      </c>
-      <c r="CC4" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="CD4" t="n">
-        <v>4.27</v>
-      </c>
-      <c r="CE4" t="n">
-        <v>4.85</v>
-      </c>
-      <c r="CF4" t="n">
-        <v>4.9</v>
-      </c>
       <c r="CG4" t="n">
-        <v>7.07</v>
+        <v>4.25</v>
       </c>
       <c r="CH4" t="n">
-        <v>0</v>
+        <v>6.33</v>
       </c>
       <c r="CI4" t="n">
-        <v>5.19</v>
+        <v>5.23</v>
       </c>
       <c r="CJ4" t="n">
+        <v>6.22</v>
+      </c>
+      <c r="CK4" t="n">
+        <v>5.34</v>
+      </c>
+      <c r="CL4" t="n">
+        <v>4.72</v>
+      </c>
+      <c r="CM4" t="n">
         <v>4.84</v>
       </c>
-      <c r="CK4" t="n">
-        <v>5.51</v>
-      </c>
-      <c r="CL4" t="n">
-        <v>5.38</v>
-      </c>
-      <c r="CM4" t="n">
-        <v>5.06</v>
-      </c>
       <c r="CN4" t="n">
-        <v>5.22</v>
+        <v>4.75</v>
       </c>
       <c r="CO4" t="n">
-        <v>5.88</v>
+        <v>4.56</v>
       </c>
       <c r="CP4" t="n">
-        <v>5.07</v>
+        <v>5.44</v>
       </c>
       <c r="CQ4" t="n">
-        <v>5.07</v>
+        <v>5.44</v>
       </c>
       <c r="CR4" t="n">
-        <v>5.77</v>
+        <v>5.26</v>
       </c>
       <c r="CS4" t="n">
-        <v>5.77</v>
+        <v>5.26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>